<commit_message>
Schulz MuK 22 mit 4 wellen
</commit_message>
<xml_diff>
--- a/script/Clpm_t4_layout.xlsx
+++ b/script/Clpm_t4_layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Daten/UNI/0_AKT/RI-CLPM_SS23/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1E2972-D310-6449-A985-C2282D3549FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7415B2FC-3402-D143-81A5-1D295135C6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18200" yWindow="8940" windowWidth="26340" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9660" yWindow="3080" windowWidth="26340" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -465,31 +465,87 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="A2">
+        <v>-99</v>
+      </c>
+      <c r="B2">
+        <v>-99</v>
+      </c>
+      <c r="C2">
+        <v>-99</v>
+      </c>
+      <c r="D2">
+        <v>-99</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>-99</v>
+      </c>
+      <c r="B4">
+        <v>-99</v>
+      </c>
+      <c r="C4">
+        <v>-99</v>
+      </c>
+      <c r="D4">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>-99</v>
+      </c>
+      <c r="B5">
+        <v>-99</v>
+      </c>
+      <c r="C5">
+        <v>-99</v>
+      </c>
+      <c r="D5">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D6" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>-99</v>
+      </c>
+      <c r="B7">
+        <v>-99</v>
+      </c>
+      <c r="C7">
+        <v>-99</v>
+      </c>
+      <c r="D7">
+        <v>-99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>